<commit_message>
Creating a test for NVivo coded comment creation.
</commit_message>
<xml_diff>
--- a/data/Sample Surveys/Better Sample Survey/Comment Coding NVivo/Q5 Coded_NVivo.xlsx
+++ b/data/Sample Surveys/Better Sample Survey/Comment Coding NVivo/Q5 Coded_NVivo.xlsx
@@ -5,19 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\Student Work\QualtricsTools\QualtricsTools R Project\QualtricsTools\data\Sample Surveys\Better Sample Survey\Comment-coding\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\Student Work\QualtricsTools\QualtricsTools R Project\QualtricsTools\data\Sample Surveys\Better Sample Survey\Comment Coding NVivo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8115D2F-5C3D-4750-9C73-F0D82D3578FF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463B5F81-7288-4444-82A2-E4EDF6A7CD55}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32445" yWindow="1575" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coded" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -133,70 +130,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Better_Sample_Survey"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>R_9RWrgh1F9m7488l</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>R_01HREuYKcsQtj5r</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>R_7U6eBR7waV8xr0N</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>R_6FsLhwCAYml5NOJ</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>R_3OCWLC3rgTT1pgF</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>R_bQ6PNClOxWzN2El</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>R_1KZoMuQosaLODnD</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>R_9WxVeTZE0AYGM3b</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>R_enxo3IGmYtlUhtX</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13" t="str">
-            <v>R_2rzdbdSqbgVTlHv</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -462,151 +395,129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="21.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" customWidth="1"/>
-    <col min="5" max="5" width="43.42578125" customWidth="1"/>
-    <col min="6" max="6" width="44.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" customWidth="1"/>
+    <col min="4" max="4" width="43.42578125" customWidth="1"/>
+    <col min="5" max="5" width="44.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="C1" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="str">
-        <f>VLOOKUP(A2,[1]Better_Sample_Survey!$A$4:$A$13,1,FALSE)</f>
-        <v>R_9RWrgh1F9m7488l</v>
-      </c>
-      <c r="C2" s="3">
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="str">
-        <f>VLOOKUP(A3,[1]Better_Sample_Survey!$A$4:$A$13,1,FALSE)</f>
-        <v>R_01HREuYKcsQtj5r</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1</v>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="str">
-        <f>VLOOKUP(A4,[1]Better_Sample_Survey!$A$4:$A$13,1,FALSE)</f>
-        <v>R_7U6eBR7waV8xr0N</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1</v>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="str">
-        <f>VLOOKUP(A5,[1]Better_Sample_Survey!$A$4:$A$13,1,FALSE)</f>
-        <v>R_6FsLhwCAYml5NOJ</v>
-      </c>
-      <c r="C5" s="3">
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5">
         <v>1</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="str">
-        <f>VLOOKUP(A6,[1]Better_Sample_Survey!$A$4:$A$13,1,FALSE)</f>
-        <v>R_3OCWLC3rgTT1pgF</v>
-      </c>
-      <c r="C6" s="3">
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6">
         <v>1</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" t="str">
-        <f>VLOOKUP(A7,[1]Better_Sample_Survey!$A$4:$A$13,1,FALSE)</f>
-        <v>R_9RWrgh1F9m7488l</v>
-      </c>
-      <c r="C7" s="3">
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
@@ -615,19 +526,15 @@
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" t="str">
-        <f>VLOOKUP(A8,[1]Better_Sample_Survey!$A$4:$A$13,1,FALSE)</f>
-        <v>R_01HREuYKcsQtj5r</v>
-      </c>
-      <c r="C8" s="3">
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
@@ -636,19 +543,15 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="str">
-        <f>VLOOKUP(A9,[1]Better_Sample_Survey!$A$4:$A$13,1,FALSE)</f>
-        <v>R_3OCWLC3rgTT1pgF</v>
-      </c>
-      <c r="C9" s="3">
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+      <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
@@ -657,19 +560,15 @@
       <c r="E9">
         <v>0</v>
       </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="str">
-        <f>VLOOKUP(A10,[1]Better_Sample_Survey!$A$4:$A$13,1,FALSE)</f>
-        <v>R_2rzdbdSqbgVTlHv</v>
-      </c>
-      <c r="C10" s="3">
+      <c r="B10" s="3">
+        <v>0</v>
+      </c>
+      <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
@@ -678,54 +577,51 @@
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C25" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>